<commit_message>
Updated Sprint Review Prot. 3
</commit_message>
<xml_diff>
--- a/Sprints/Sprint3/Sprint_Review_3.xlsx
+++ b/Sprints/Sprint3/Sprint_Review_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farha\Documents\Studium\LVs\ITP\GithubRep\ProjectWebshop\Sprints\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C61A7D5-9C65-490B-8906-1173E574035A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3F1033-0937-4228-8026-541869B28018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5805" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
@@ -407,6 +407,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -425,12 +443,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,18 +466,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE3C726-37E9-451B-9308-D99ECF6E7468}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -800,28 +800,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -835,131 +835,131 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="18">
+      <c r="A4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22">
         <v>3</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="24" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1000,7 +1000,9 @@
         <f>D16-C16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
     </row>
@@ -1040,7 +1042,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
@@ -1051,13 +1055,19 @@
       <c r="B19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="C19" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="D19" s="7">
+        <v>2</v>
+      </c>
       <c r="E19" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>-0.5</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
@@ -1068,13 +1078,19 @@
       <c r="B20" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1.5</v>
+      </c>
       <c r="E20" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="7"/>
     </row>
@@ -1085,13 +1101,17 @@
       <c r="B21" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="7">
+        <v>1.5</v>
+      </c>
       <c r="D21" s="7"/>
       <c r="E21" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="3"/>
+        <v>-1.5</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
@@ -1102,13 +1122,17 @@
       <c r="B22" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="7">
+        <v>1.5</v>
+      </c>
       <c r="D22" s="7"/>
       <c r="E22" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
+        <v>-1.5</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
@@ -1119,13 +1143,19 @@
       <c r="B23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="C23" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
       <c r="E23" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="3"/>
+        <v>-0.5</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
@@ -1159,13 +1189,19 @@
       <c r="B25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1.5</v>
+      </c>
       <c r="E25" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
@@ -1176,13 +1212,19 @@
       <c r="B26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="C26" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E26" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="3"/>
+        <v>-2</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
       <c r="G26" s="4"/>
       <c r="H26" s="7"/>
     </row>
@@ -1193,13 +1235,19 @@
       <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="C27" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E27" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="3"/>
+        <v>-2</v>
+      </c>
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="7"/>
     </row>
@@ -1210,13 +1258,19 @@
       <c r="B28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0.25</v>
+      </c>
       <c r="E28" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="3"/>
+        <v>-0.75</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="7"/>
     </row>
@@ -1290,11 +1344,11 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6">
         <f>SUM(E16:E32)</f>
-        <v>0</v>
+        <v>-7.75</v>
       </c>
       <c r="F33" s="6">
         <f>COUNT(F16:F32)</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G33" s="6">
         <f>COUNT(G16:G32)</f>
@@ -1315,11 +1369,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1334,6 +1383,11 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
     <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>